<commit_message>
20150603 - swap TIM1/TIM4 functions on AQ32 target
(to better align with AQ32 pin usage.)

Author is jihlein, mlyle removed board-orientation related changes.
</commit_message>
<xml_diff>
--- a/flight/targets/aq32/hw/aq32Taulabs.xlsx
+++ b/flight/targets/aq32/hw/aq32Taulabs.xlsx
@@ -816,9 +816,6 @@
     <t>GPS RX (USART2 RX)</t>
   </si>
   <si>
-    <t>AQ32 Use</t>
-  </si>
-  <si>
     <t>ESC PWM3 (TIM8 CH2)</t>
   </si>
   <si>
@@ -1161,9 +1158,6 @@
     <t>Spektrum Parser</t>
   </si>
   <si>
-    <t>TauLabs Use</t>
-  </si>
-  <si>
     <t>UART 6 TX</t>
   </si>
   <si>
@@ -1227,24 +1221,6 @@
     <t>UART3 RX</t>
   </si>
   <si>
-    <t>PWM Out 9 (TIM4 CH1)</t>
-  </si>
-  <si>
-    <t>PWM Out 12 (TIM4 CH4)</t>
-  </si>
-  <si>
-    <t>PWM Out 10 (TIM4 CH2)</t>
-  </si>
-  <si>
-    <t>PWM Out 11 (TIM4 CH3)</t>
-  </si>
-  <si>
-    <t>Serial PPM (TIM1 CH4)</t>
-  </si>
-  <si>
-    <t>RangeFinder (TIM1 CH3)</t>
-  </si>
-  <si>
     <t>Heartbeat LED</t>
   </si>
   <si>
@@ -1258,6 +1234,30 @@
   </si>
   <si>
     <t>ADC2, External Current Monitor</t>
+  </si>
+  <si>
+    <t>PPM (TIM4 CH1)</t>
+  </si>
+  <si>
+    <t>RangeFinder (TIM4 CH2)</t>
+  </si>
+  <si>
+    <t>PWM Out 9 (TIM1 CH1)</t>
+  </si>
+  <si>
+    <t>PWM Out 10 (TIM1 CH2)</t>
+  </si>
+  <si>
+    <t>PWM Out 11 (TIM1 CH3)</t>
+  </si>
+  <si>
+    <t>PWM Out 12 (TIM1 CH4)</t>
+  </si>
+  <si>
+    <t>AQ32 Definition</t>
+  </si>
+  <si>
+    <t>TauLabs Definition</t>
   </si>
 </sst>
 </file>
@@ -1747,7 +1747,7 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1771,28 +1771,28 @@
         <v>246</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>258</v>
+        <v>404</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>373</v>
+        <v>405</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>246</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>258</v>
+        <v>404</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>373</v>
+        <v>405</v>
       </c>
       <c r="I1" s="19" t="s">
         <v>246</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>258</v>
+        <v>404</v>
       </c>
       <c r="K1" s="19" t="s">
-        <v>373</v>
+        <v>405</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1800,19 +1800,19 @@
         <v>134</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E2" s="21" t="s">
         <v>166</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="I2" s="21" t="s">
         <v>198</v>
@@ -1826,10 +1826,10 @@
         <v>135</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E3" s="21" t="s">
         <v>167</v>
@@ -1846,16 +1846,16 @@
         <v>136</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>168</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I4" s="21" t="s">
         <v>200</v>
@@ -1869,7 +1869,7 @@
         <v>169</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I5" s="21" t="s">
         <v>201</v>
@@ -1886,7 +1886,7 @@
         <v>67</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="I6" s="21" t="s">
         <v>202</v>
@@ -1903,10 +1903,10 @@
         <v>171</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="I7" s="21" t="s">
         <v>203</v>
@@ -1915,7 +1915,7 @@
         <v>217</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1929,10 +1929,10 @@
         <v>172</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="I8" s="21" t="s">
         <v>204</v>
@@ -1941,7 +1941,7 @@
         <v>218</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1955,10 +1955,10 @@
         <v>173</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="I9" s="21" t="s">
         <v>205</v>
@@ -1975,7 +1975,7 @@
         <v>224</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="I10" s="21" t="s">
         <v>206</v>
@@ -1989,7 +1989,7 @@
         <v>234</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E11" s="21" t="s">
         <v>175</v>
@@ -1998,13 +1998,16 @@
         <v>223</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I11" s="21" t="s">
         <v>207</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>277</v>
+        <v>276</v>
+      </c>
+      <c r="K11" s="17" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -2015,7 +2018,7 @@
         <v>235</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>176</v>
@@ -2038,7 +2041,7 @@
         <v>247</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E13" s="21" t="s">
         <v>177</v>
@@ -2053,7 +2056,10 @@
         <v>209</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>278</v>
+        <v>277</v>
+      </c>
+      <c r="K13" s="17" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -2064,7 +2070,7 @@
         <v>248</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E14" s="21" t="s">
         <v>178</v>
@@ -2096,10 +2102,10 @@
         <v>211</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -2119,10 +2125,10 @@
         <v>212</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -2130,10 +2136,10 @@
         <v>149</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E17" s="21" t="s">
         <v>181</v>
@@ -2147,7 +2153,7 @@
         <v>150</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E19" s="21" t="s">
         <v>182</v>
@@ -2177,10 +2183,10 @@
         <v>153</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E22" s="21" t="s">
         <v>185</v>
@@ -2191,10 +2197,10 @@
         <v>154</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E23" s="21" t="s">
         <v>186</v>
@@ -2208,10 +2214,10 @@
         <v>155</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E24" s="21" t="s">
         <v>187</v>
@@ -2220,7 +2226,7 @@
         <v>256</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -2240,7 +2246,7 @@
         <v>257</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -2277,10 +2283,10 @@
         <v>190</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -2291,10 +2297,10 @@
         <v>191</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -2302,10 +2308,10 @@
         <v>160</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E29" s="21" t="s">
         <v>192</v>
@@ -2316,10 +2322,10 @@
         <v>161</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E30" s="21" t="s">
         <v>193</v>
@@ -2339,10 +2345,10 @@
         <v>194</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -2356,13 +2362,13 @@
         <v>195</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="21" t="s">
         <v>164</v>
       </c>
@@ -2373,13 +2379,10 @@
         <v>196</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>275</v>
-      </c>
-      <c r="G33" s="17" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="21" t="s">
         <v>165</v>
       </c>
@@ -2390,10 +2393,7 @@
         <v>197</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>276</v>
-      </c>
-      <c r="G34" s="17" t="s">
-        <v>396</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -2600,7 +2600,7 @@
         <v>118</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -3184,7 +3184,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1">
       <c r="A1" s="13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>100</v>
@@ -3192,77 +3192,77 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C16" t="s">
         <v>119</v>
@@ -3270,17 +3270,17 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="18" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C19" t="s">
         <v>118</v>
@@ -3288,283 +3288,283 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="18" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C29" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C33" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="18" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C34" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="18" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C35" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="18" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C36" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="18" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C54" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="18" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C56" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="18" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C71" t="s">
         <v>122</v>
@@ -3572,7 +3572,7 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="18" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C72" t="s">
         <v>117</v>
@@ -3580,60 +3580,60 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C73" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20150715 - Update AQ32 pin definition file in hardware folder.
</commit_message>
<xml_diff>
--- a/flight/targets/aq32/hw/aq32Taulabs.xlsx
+++ b/flight/targets/aq32/hw/aq32Taulabs.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="404">
   <si>
     <t>DMA1 Request Mapping</t>
   </si>
@@ -1173,12 +1173,6 @@
     <t>UART4 RX</t>
   </si>
   <si>
-    <t>PWM Out 8 (TIM5 CH3)</t>
-  </si>
-  <si>
-    <t>PWM Out 7 (TIM5 CH1)</t>
-  </si>
-  <si>
     <t>UART1 TX</t>
   </si>
   <si>
@@ -1239,25 +1233,25 @@
     <t>PPM (TIM4 CH1)</t>
   </si>
   <si>
-    <t>RangeFinder (TIM4 CH2)</t>
-  </si>
-  <si>
-    <t>PWM Out 9 (TIM1 CH1)</t>
-  </si>
-  <si>
-    <t>PWM Out 10 (TIM1 CH2)</t>
-  </si>
-  <si>
-    <t>PWM Out 11 (TIM1 CH3)</t>
-  </si>
-  <si>
-    <t>PWM Out 12 (TIM1 CH4)</t>
-  </si>
-  <si>
     <t>AQ32 Definition</t>
   </si>
   <si>
     <t>TauLabs Definition</t>
+  </si>
+  <si>
+    <t>UART4 TX</t>
+  </si>
+  <si>
+    <t>PWM Out 7 (TIM1 CH1)</t>
+  </si>
+  <si>
+    <t>PWM Out 8 (TIM1 CH2)</t>
+  </si>
+  <si>
+    <t>PWM Out 9 (TIM1 CH3)</t>
+  </si>
+  <si>
+    <t>PWM Out 10 (TIM1 CH4)</t>
   </si>
 </sst>
 </file>
@@ -1746,8 +1740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1771,28 +1765,28 @@
         <v>246</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>246</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="I1" s="19" t="s">
         <v>246</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="K1" s="19" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1803,7 +1797,7 @@
         <v>261</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>378</v>
+        <v>399</v>
       </c>
       <c r="E2" s="21" t="s">
         <v>166</v>
@@ -1812,7 +1806,7 @@
         <v>271</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="I2" s="21" t="s">
         <v>198</v>
@@ -1848,9 +1842,6 @@
       <c r="B4" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>377</v>
-      </c>
       <c r="E4" s="21" t="s">
         <v>168</v>
       </c>
@@ -1886,7 +1877,7 @@
         <v>67</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I6" s="21" t="s">
         <v>202</v>
@@ -1906,7 +1897,7 @@
         <v>268</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I7" s="21" t="s">
         <v>203</v>
@@ -1915,7 +1906,7 @@
         <v>217</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1941,7 +1932,7 @@
         <v>218</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1975,7 +1966,7 @@
         <v>224</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="I10" s="21" t="s">
         <v>206</v>
@@ -1989,7 +1980,7 @@
         <v>234</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E11" s="21" t="s">
         <v>175</v>
@@ -1998,7 +1989,7 @@
         <v>223</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="I11" s="21" t="s">
         <v>207</v>
@@ -2018,7 +2009,7 @@
         <v>235</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>176</v>
@@ -2041,7 +2032,7 @@
         <v>247</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E13" s="21" t="s">
         <v>177</v>
@@ -2070,7 +2061,7 @@
         <v>248</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E14" s="21" t="s">
         <v>178</v>
@@ -2139,7 +2130,7 @@
         <v>263</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E17" s="21" t="s">
         <v>181</v>
@@ -2186,7 +2177,7 @@
         <v>264</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E22" s="21" t="s">
         <v>185</v>
@@ -2200,7 +2191,7 @@
         <v>265</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E23" s="21" t="s">
         <v>186</v>
@@ -2217,7 +2208,7 @@
         <v>266</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E24" s="21" t="s">
         <v>187</v>
@@ -2283,10 +2274,10 @@
         <v>190</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -2297,10 +2288,10 @@
         <v>191</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -2308,10 +2299,10 @@
         <v>160</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E29" s="21" t="s">
         <v>192</v>
@@ -2322,10 +2313,10 @@
         <v>161</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E30" s="21" t="s">
         <v>193</v>
@@ -2347,9 +2338,6 @@
       <c r="F31" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="G31" s="17" t="s">
-        <v>398</v>
-      </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="21" t="s">
@@ -2364,11 +2352,8 @@
       <c r="F32" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="G32" s="17" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="21" t="s">
         <v>164</v>
       </c>
@@ -2382,7 +2367,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:7">
       <c r="A34" s="21" t="s">
         <v>165</v>
       </c>
@@ -2394,6 +2379,9 @@
       </c>
       <c r="F34" s="17" t="s">
         <v>275</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>396</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20150721 - Updated the pin definitions.
</commit_message>
<xml_diff>
--- a/flight/targets/aq32/hw/aq32Taulabs.xlsx
+++ b/flight/targets/aq32/hw/aq32Taulabs.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="407">
   <si>
     <t>DMA1 Request Mapping</t>
   </si>
@@ -1230,9 +1230,6 @@
     <t>ADC2, External Current Monitor</t>
   </si>
   <si>
-    <t>PPM (TIM4 CH1)</t>
-  </si>
-  <si>
     <t>AQ32 Definition</t>
   </si>
   <si>
@@ -1242,16 +1239,28 @@
     <t>UART4 TX</t>
   </si>
   <si>
-    <t>PWM Out 7 (TIM1 CH1)</t>
-  </si>
-  <si>
-    <t>PWM Out 8 (TIM1 CH2)</t>
-  </si>
-  <si>
-    <t>PWM Out 9 (TIM1 CH3)</t>
-  </si>
-  <si>
-    <t>PWM Out 10 (TIM1 CH4)</t>
+    <t>PWM In 4/PPM</t>
+  </si>
+  <si>
+    <t>PWM In 1</t>
+  </si>
+  <si>
+    <t>PWM In 2</t>
+  </si>
+  <si>
+    <t>PWM In 3</t>
+  </si>
+  <si>
+    <t>PWM In 5/PWM Out 7</t>
+  </si>
+  <si>
+    <t>PWM In 6/PWM Out 8</t>
+  </si>
+  <si>
+    <t>PWM In 7/PWM Out 9</t>
+  </si>
+  <si>
+    <t>PWM In 8/PWM Out 10</t>
   </si>
 </sst>
 </file>
@@ -1740,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1765,28 +1774,28 @@
         <v>246</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>396</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>397</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>398</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>246</v>
       </c>
       <c r="F1" s="19" t="s">
+        <v>396</v>
+      </c>
+      <c r="G1" s="19" t="s">
         <v>397</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>398</v>
       </c>
       <c r="I1" s="19" t="s">
         <v>246</v>
       </c>
       <c r="J1" s="19" t="s">
+        <v>396</v>
+      </c>
+      <c r="K1" s="19" t="s">
         <v>397</v>
-      </c>
-      <c r="K1" s="19" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1797,7 +1806,7 @@
         <v>261</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E2" s="21" t="s">
         <v>166</v>
@@ -1998,7 +2007,7 @@
         <v>276</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -2050,7 +2059,7 @@
         <v>277</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -2096,7 +2105,7 @@
         <v>278</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -2119,7 +2128,7 @@
         <v>279</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -2338,6 +2347,9 @@
       <c r="F31" s="17" t="s">
         <v>272</v>
       </c>
+      <c r="G31" s="17" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="21" t="s">
@@ -2352,6 +2364,9 @@
       <c r="F32" s="17" t="s">
         <v>273</v>
       </c>
+      <c r="G32" s="17" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="21" t="s">
@@ -2366,6 +2381,9 @@
       <c r="F33" s="17" t="s">
         <v>274</v>
       </c>
+      <c r="G33" s="17" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="21" t="s">
@@ -2381,7 +2399,7 @@
         <v>275</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20150723 - Code cleanup, fomatting cleanup, add SPI1 and SPI2 pin definitions.
</commit_message>
<xml_diff>
--- a/flight/targets/aq32/hw/aq32Taulabs.xlsx
+++ b/flight/targets/aq32/hw/aq32Taulabs.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="410">
   <si>
     <t>DMA1 Request Mapping</t>
   </si>
@@ -1261,6 +1261,15 @@
   </si>
   <si>
     <t>PWM In 8/PWM Out 10</t>
+  </si>
+  <si>
+    <t>SD Card CS</t>
+  </si>
+  <si>
+    <t>SP12 CS</t>
+  </si>
+  <si>
+    <t>SPI2 CS</t>
   </si>
 </sst>
 </file>
@@ -1749,8 +1758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1865,6 +1874,12 @@
       <c r="A5" s="21" t="s">
         <v>137</v>
       </c>
+      <c r="B5" s="17" t="s">
+        <v>408</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>409</v>
+      </c>
       <c r="E5" s="21" t="s">
         <v>169</v>
       </c>
@@ -1899,6 +1914,9 @@
       <c r="B7" s="17" t="s">
         <v>225</v>
       </c>
+      <c r="C7" s="17" t="s">
+        <v>225</v>
+      </c>
       <c r="E7" s="21" t="s">
         <v>171</v>
       </c>
@@ -1925,6 +1943,9 @@
       <c r="B8" s="17" t="s">
         <v>226</v>
       </c>
+      <c r="C8" s="17" t="s">
+        <v>226</v>
+      </c>
       <c r="E8" s="21" t="s">
         <v>172</v>
       </c>
@@ -1951,6 +1972,9 @@
       <c r="B9" s="17" t="s">
         <v>227</v>
       </c>
+      <c r="C9" s="17" t="s">
+        <v>227</v>
+      </c>
       <c r="E9" s="21" t="s">
         <v>173</v>
       </c>
@@ -2032,6 +2056,12 @@
       <c r="I12" s="21" t="s">
         <v>208</v>
       </c>
+      <c r="J12" s="17" t="s">
+        <v>407</v>
+      </c>
+      <c r="K12" s="17" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="21" t="s">
@@ -2358,6 +2388,9 @@
       <c r="B32" s="17" t="s">
         <v>228</v>
       </c>
+      <c r="C32" s="17" t="s">
+        <v>228</v>
+      </c>
       <c r="E32" s="21" t="s">
         <v>195</v>
       </c>
@@ -2375,6 +2408,9 @@
       <c r="B33" s="17" t="s">
         <v>229</v>
       </c>
+      <c r="C33" s="17" t="s">
+        <v>229</v>
+      </c>
       <c r="E33" s="21" t="s">
         <v>196</v>
       </c>
@@ -2390,6 +2426,9 @@
         <v>165</v>
       </c>
       <c r="B34" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>230</v>
       </c>
       <c r="E34" s="21" t="s">

</xml_diff>